<commit_message>
CIERRE 16 MAR 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #03  MARZO  2022/CREDITOS  4 CARNES   ZAVALETA   MaRzO   2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #03  MARZO  2022/CREDITOS  4 CARNES   ZAVALETA   MaRzO   2022.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="36">
   <si>
     <t>REMISION</t>
   </si>
@@ -9033,7 +9033,7 @@
   <dimension ref="A1:I74"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10601,8 +10601,8 @@
   </sheetPr>
   <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10875,11 +10875,15 @@
       <c r="E13" s="20">
         <v>28638</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="22"/>
+      <c r="F13" s="21">
+        <v>44632</v>
+      </c>
+      <c r="G13" s="22">
+        <v>28638</v>
+      </c>
       <c r="H13" s="18">
         <f t="shared" si="0"/>
-        <v>28638</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -11051,93 +11055,129 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+      <c r="A22" s="12">
+        <v>44632</v>
+      </c>
       <c r="B22" s="13">
         <v>249</v>
       </c>
       <c r="C22" s="24"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="20"/>
+      <c r="D22" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="20">
+        <v>8120</v>
+      </c>
       <c r="F22" s="21"/>
       <c r="G22" s="22"/>
       <c r="H22" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8120</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="12">
+        <v>44632</v>
+      </c>
       <c r="B23" s="13">
         <v>250</v>
       </c>
       <c r="C23" s="24"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20"/>
+      <c r="D23" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="20">
+        <v>50260</v>
+      </c>
       <c r="F23" s="21"/>
       <c r="G23" s="22"/>
       <c r="H23" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>50260</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
+      <c r="A24" s="12">
+        <v>44633</v>
+      </c>
       <c r="B24" s="13">
         <v>251</v>
       </c>
       <c r="C24" s="24"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="20"/>
+      <c r="D24" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="20">
+        <v>84535</v>
+      </c>
       <c r="F24" s="21"/>
       <c r="G24" s="22"/>
       <c r="H24" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>84535</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
+      <c r="A25" s="12">
+        <v>44633</v>
+      </c>
       <c r="B25" s="13">
         <v>252</v>
       </c>
       <c r="C25" s="24"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="20"/>
+      <c r="D25" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="20">
+        <v>77384</v>
+      </c>
       <c r="F25" s="21"/>
       <c r="G25" s="22"/>
       <c r="H25" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>77384</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
+      <c r="A26" s="12">
+        <v>44633</v>
+      </c>
       <c r="B26" s="13">
         <v>253</v>
       </c>
       <c r="C26" s="24"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="20"/>
+      <c r="D26" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="20">
+        <v>71425</v>
+      </c>
       <c r="F26" s="21"/>
       <c r="G26" s="22"/>
       <c r="H26" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>71425</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
+      <c r="A27" s="12">
+        <v>44633</v>
+      </c>
       <c r="B27" s="13">
         <v>254</v>
       </c>
       <c r="C27" s="24"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="20"/>
+      <c r="D27" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="20">
+        <v>2969</v>
+      </c>
       <c r="F27" s="21"/>
       <c r="G27" s="22"/>
       <c r="H27" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2969</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -11686,16 +11726,16 @@
       <c r="D64" s="2"/>
       <c r="E64" s="39">
         <f>SUM(E4:E63)</f>
-        <v>330661</v>
+        <v>625354</v>
       </c>
       <c r="F64" s="39"/>
       <c r="G64" s="39">
         <f>SUM(G4:G63)</f>
-        <v>1827</v>
+        <v>30465</v>
       </c>
       <c r="H64" s="40">
         <f>SUM(H4:H63)</f>
-        <v>328834</v>
+        <v>594889</v>
       </c>
       <c r="I64" s="2"/>
     </row>
@@ -11739,7 +11779,7 @@
       <c r="D68" s="2"/>
       <c r="E68" s="110">
         <f>E64-G64</f>
-        <v>328834</v>
+        <v>594889</v>
       </c>
       <c r="F68" s="111"/>
       <c r="G68" s="112"/>

</xml_diff>